<commit_message>
I made look more beautiful.
</commit_message>
<xml_diff>
--- a/BernalPabloGraphics2Project/Dev IV Project Rubric.xlsx
+++ b/BernalPabloGraphics2Project/Dev IV Project Rubric.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -891,7 +891,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E71,"=I",G4:G71) + SUMIF(C73:C74, "X",B73:B74) &gt; 18, 18, SUMIF(E4:E71,"=I",G4:G71) + SUMIF(C73:C74, "X",B73:B74))</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74) &gt; 18, 18, SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74))</f>
@@ -1031,11 +1031,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G71) + SUMIF(C73:C74, "X",B73:B74) + SUMIF(D73:D74, "X",B73:B74) + SUMIF(E73:E74, "X",B73:B74)</f>
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E71,"=I",G4:G71) + SUMIF(C73:C74, "X",B73:B74)  &gt; 18, SUMIF(E4:E71,"=I",G4:G71) + SUMIF(C73:C74, "X",B73:B74) - 18,0)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74) &gt; 18, SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74) - 18,0)</f>
@@ -1164,11 +1164,11 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
@@ -1369,11 +1369,15 @@
       <c r="D17" s="5">
         <v>2</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G17" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1547,11 +1551,15 @@
       <c r="D25" s="5">
         <v>2</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
+      <c r="E25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G25" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1572,11 +1580,15 @@
       <c r="D26" s="5">
         <v>2</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
+      <c r="E26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G26" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1597,11 +1609,15 @@
       <c r="D27" s="5">
         <v>2</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="3"/>
+      <c r="E27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G27" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -1622,11 +1638,15 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -2590,7 +2610,9 @@
       <c r="B73" s="6">
         <v>2</v>
       </c>
-      <c r="C73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="5"/>
@@ -2608,7 +2630,9 @@
       <c r="B74" s="6">
         <v>1</v>
       </c>
-      <c r="C74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="5"/>
@@ -2743,7 +2767,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Cube with textures added
</commit_message>
<xml_diff>
--- a/BernalPabloGraphics2Project/Dev IV Project Rubric.xlsx
+++ b/BernalPabloGraphics2Project/Dev IV Project Rubric.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Student Git Address: https://github.com/PabloBernalAlarcon/GX2ProhectRepo.git</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -891,7 +894,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1026,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74) &gt; 18, 18, SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E71,"=III",G4:G71) + SUMIF(E73:E74, "X",B73:B74) &gt; 18, 18, SUMIF(E4:E71,"=III",G4:G71) + SUMIF(E73:E74, "X",B73:B74))</f>
@@ -1035,7 +1038,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G71) + SUMIF(C73:C74, "X",B73:B74) + SUMIF(D73:D74, "X",B73:B74) + SUMIF(E73:E74, "X",B73:B74)</f>
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1088,11 +1091,15 @@
       <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E71,"=I",G4:G71) + SUMIF(C73:C74, "X",B73:B74)  &gt; 18, SUMIF(E4:E71,"=I",G4:G71) + SUMIF(C73:C74, "X",B73:B74) - 18,0)</f>
@@ -1168,7 +1175,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1448,7 +1455,9 @@
       <c r="D20" s="5">
         <v>3</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="16">
         <f t="shared" si="0"/>
@@ -1667,7 +1676,9 @@
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
@@ -1692,7 +1703,9 @@
       <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
@@ -1717,7 +1730,9 @@
       <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="16">
         <f t="shared" ref="G31:G55" si="1" xml:space="preserve"> IF(EXACT(F31,"X"),IF(EXACT(E31,"I"),$B31,IF(EXACT(E31,"II"),$C31,IF(EXACT(E31,"III"),$D31,0))),0)</f>
@@ -2048,7 +2063,9 @@
       <c r="D46" s="5">
         <v>2</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F46" s="3"/>
       <c r="G46" s="16">
         <f t="shared" si="1"/>
@@ -2073,7 +2090,9 @@
       <c r="D47" s="5">
         <v>3</v>
       </c>
-      <c r="E47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F47" s="3"/>
       <c r="G47" s="16">
         <f t="shared" si="1"/>
@@ -2176,7 +2195,9 @@
       <c r="D52" s="5">
         <v>1</v>
       </c>
-      <c r="E52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F52" s="3"/>
       <c r="G52" s="16">
         <f t="shared" si="1"/>
@@ -2251,7 +2272,9 @@
       <c r="D55" s="5">
         <v>4</v>
       </c>
-      <c r="E55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="F55" s="3"/>
       <c r="G55" s="16">
         <f t="shared" si="1"/>
@@ -2613,7 +2636,9 @@
       <c r="C73" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D73" s="3"/>
+      <c r="D73" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="E73" s="3"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
@@ -2633,7 +2658,9 @@
       <c r="C74" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D74" s="3"/>
+      <c r="D74" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="E74" s="3"/>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
@@ -2767,7 +2794,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Milestone 2 done, for real
</commit_message>
<xml_diff>
--- a/BernalPabloGraphics2Project/Dev IV Project Rubric.xlsx
+++ b/BernalPabloGraphics2Project/Dev IV Project Rubric.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -341,9 +341,6 @@
   </si>
   <si>
     <t>II</t>
-  </si>
-  <si>
-    <t>III</t>
   </si>
 </sst>
 </file>
@@ -896,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1679,9 +1676,7 @@
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="E29" s="2"/>
       <c r="F29" s="3"/>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
@@ -1706,9 +1701,7 @@
       <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="E30" s="2"/>
       <c r="F30" s="3"/>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
@@ -1733,9 +1726,7 @@
       <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="E31" s="2"/>
       <c r="F31" s="3"/>
       <c r="G31" s="16">
         <f t="shared" ref="G31:G55" si="1" xml:space="preserve"> IF(EXACT(F31,"X"),IF(EXACT(E31,"I"),$B31,IF(EXACT(E31,"II"),$C31,IF(EXACT(E31,"III"),$D31,0))),0)</f>
@@ -2202,9 +2193,7 @@
       <c r="D52" s="5">
         <v>1</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="E52" s="2"/>
       <c r="F52" s="3"/>
       <c r="G52" s="16">
         <f t="shared" si="1"/>
@@ -2279,9 +2268,7 @@
       <c r="D55" s="5">
         <v>4</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="E55" s="2"/>
       <c r="F55" s="3"/>
       <c r="G55" s="16">
         <f t="shared" si="1"/>
@@ -2441,9 +2428,7 @@
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
-      <c r="E63" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="E63" s="2"/>
       <c r="F63" s="3"/>
       <c r="G63" s="16">
         <f t="shared" ref="G63:G68" si="3" xml:space="preserve"> IF(EXACT(F63,"X"),IF(EXACT(E63,"I"),$B63,IF(EXACT(E63,"II"),$C63,IF(EXACT(E63,"III"),$D63,0))),0)</f>
@@ -2807,7 +2792,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
okay, this is the last one
</commit_message>
<xml_diff>
--- a/BernalPabloGraphics2Project/Dev IV Project Rubric.xlsx
+++ b/BernalPabloGraphics2Project/Dev IV Project Rubric.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="88">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E71,"=III",G4:G71) + SUMIF(E73:E74, "X",B73:B74) &gt; 18, 18, SUMIF(E4:E71,"=III",G4:G71) + SUMIF(E73:E74, "X",B73:B74))</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G71) + SUMIF(C73:C74, "X",B73:B74) + SUMIF(D73:D74, "X",B73:B74) + SUMIF(E73:E74, "X",B73:B74)</f>
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1115,7 +1115,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2210,11 +2210,15 @@
       <c r="D52" s="5">
         <v>1</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="3"/>
+      <c r="E52" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G52" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
@@ -2260,11 +2264,15 @@
       <c r="D54" s="5">
         <v>1</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="3"/>
+      <c r="E54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G54" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -2821,7 +2829,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>